<commit_message>
feat : emum 자동생성
</commit_message>
<xml_diff>
--- a/Assets/DataTable/Data.xlsx
+++ b/Assets/DataTable/Data.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SPClub\CodeLike\Assets\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8606390-7999-4018-B70B-AA0275585A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AACF94B-B4D6-40F8-8F43-E45A281271AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="EnemyData" sheetId="1" r:id="rId1"/>
-    <sheet name="DestinyData" sheetId="2" r:id="rId2"/>
-    <sheet name="DestinyEffectData" sheetId="6" r:id="rId3"/>
-    <sheet name="ActiveItemData" sheetId="5" r:id="rId4"/>
-    <sheet name="EnhanceData" sheetId="3" r:id="rId5"/>
-    <sheet name="ItemData" sheetId="4" r:id="rId6"/>
-    <sheet name="Enums" sheetId="7" r:id="rId7"/>
+    <sheet name="Enums" sheetId="7" r:id="rId1"/>
+    <sheet name="EnemyData" sheetId="1" r:id="rId2"/>
+    <sheet name="DestinyData" sheetId="2" r:id="rId3"/>
+    <sheet name="DestinyEffectData" sheetId="6" r:id="rId4"/>
+    <sheet name="ActiveItemData" sheetId="5" r:id="rId5"/>
+    <sheet name="EnhanceData" sheetId="3" r:id="rId6"/>
+    <sheet name="ItemData" sheetId="4" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="EnumGroup">Enums!$A:$A</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -103,6 +106,16 @@
   </si>
   <si>
     <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>EnumGroup</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -447,11 +460,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24A16A2-675D-4491-95B8-650037D970BC}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="A3:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="3" max="3" width="12.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -553,12 +615,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F69D4C3-5437-484D-ACFE-4ACF45820DD6}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="Q22" sqref="P22:Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -626,12 +688,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93FF34C-3225-4BA8-ACE7-B2F084BF60E3}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J27" sqref="J26:J27"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -679,7 +741,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF2F1DE-C499-42C0-9AF5-F928DBDC5D56}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -720,7 +782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FAFAE33-B027-4C65-9798-1057D5391CE0}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -761,12 +823,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{179F7B6E-E6C6-4CBE-98EC-CA5575BAAC39}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -800,20 +862,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24A16A2-675D-4491-95B8-650037D970BC}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
feat : 인벤토리 UI
</commit_message>
<xml_diff>
--- a/Assets/DataTable/Data.xlsx
+++ b/Assets/DataTable/Data.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SPClub\CodeLike\Assets\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACDE3A7-BFAC-4A2D-88E0-4D4E0E0669BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591B2B89-F449-4A7E-A246-2E2F8E91F925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Enums" sheetId="7" r:id="rId1"/>
-    <sheet name="EnemyData" sheetId="1" r:id="rId2"/>
-    <sheet name="DestinyData" sheetId="2" r:id="rId3"/>
-    <sheet name="DestinyEffectData" sheetId="6" r:id="rId4"/>
-    <sheet name="ActiveItemData" sheetId="5" r:id="rId5"/>
-    <sheet name="EnhanceData" sheetId="3" r:id="rId6"/>
-    <sheet name="ItemData" sheetId="4" r:id="rId7"/>
+    <sheet name="Table_role" sheetId="8" r:id="rId1"/>
+    <sheet name="Enums" sheetId="7" r:id="rId2"/>
+    <sheet name="EnemyData" sheetId="1" r:id="rId3"/>
+    <sheet name="DestinyData" sheetId="2" r:id="rId4"/>
+    <sheet name="DestinyEffectData" sheetId="6" r:id="rId5"/>
+    <sheet name="ActiveItemData" sheetId="5" r:id="rId6"/>
+    <sheet name="EnhanceData" sheetId="3" r:id="rId7"/>
+    <sheet name="ItemData" sheetId="4" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="EnumGroup">Enums!$A:$A</definedName>
@@ -460,10 +461,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F661DDA-2C94-4E1F-800F-48DD89B553FA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24A16A2-675D-4491-95B8-650037D970BC}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -508,12 +523,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U10" sqref="U10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -615,7 +630,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F69D4C3-5437-484D-ACFE-4ACF45820DD6}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -688,7 +703,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93FF34C-3225-4BA8-ACE7-B2F084BF60E3}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -741,7 +756,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF2F1DE-C499-42C0-9AF5-F928DBDC5D56}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -782,7 +797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FAFAE33-B027-4C65-9798-1057D5391CE0}">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -823,7 +838,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{179F7B6E-E6C6-4CBE-98EC-CA5575BAAC39}">
   <dimension ref="A1:A5"/>
   <sheetViews>

</xml_diff>

<commit_message>
feat : Condition 관련 테이블 생성
 Condition 관련 테이블 생성
 Condition 데이터 받기
</commit_message>
<xml_diff>
--- a/Assets/DataTable/Data.xlsx
+++ b/Assets/DataTable/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SPClub\CodeLike\Assets\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591B2B89-F449-4A7E-A246-2E2F8E91F925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CF3D3E-012C-43C4-A432-896F3A89F010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6570" yWindow="0" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table_role" sheetId="8" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,10 +62,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Speed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -74,10 +70,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ATK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>운명1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -118,13 +110,52 @@
   <si>
     <t>EnumGroup</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ChaseRange</t>
+  </si>
+  <si>
+    <t>Stamina</t>
+  </si>
+  <si>
+    <t>StaminaRegen</t>
+  </si>
+  <si>
+    <t>AttackPower</t>
+  </si>
+  <si>
+    <t>AttackSpeed</t>
+  </si>
+  <si>
+    <t>AttackRange</t>
+  </si>
+  <si>
+    <t>Defense</t>
+  </si>
+  <si>
+    <t>MoveSpeed</t>
+  </si>
+  <si>
+    <t>JumpPower</t>
+  </si>
+  <si>
+    <t>CriticalChance</t>
+  </si>
+  <si>
+    <t>CriticalDamage</t>
+  </si>
+  <si>
+    <t>PatrolRange</t>
+  </si>
+  <si>
+    <t>float</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,16 +178,41 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFDCDCDC"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF57A64A"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="맑은고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -164,11 +220,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -176,11 +247,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,9 +548,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F661DDA-2C94-4E1F-800F-48DD89B553FA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -482,27 +568,27 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="3" max="3" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -525,103 +611,294 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="5" max="5" width="21.875" customWidth="1"/>
+    <col min="6" max="7" width="18.375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="D1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>30</v>
-      </c>
-      <c r="D3" s="1">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="D2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9">
+        <v>1</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
+        <v>1</v>
+      </c>
+      <c r="K3" s="7">
+        <v>1</v>
+      </c>
+      <c r="L3" s="7">
+        <v>1</v>
+      </c>
+      <c r="M3" s="7">
+        <v>1</v>
+      </c>
+      <c r="N3" s="7">
+        <v>1</v>
+      </c>
+      <c r="O3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="1">
-        <v>50</v>
-      </c>
-      <c r="D4" s="1">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="C4" s="9">
+        <v>1</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
+        <v>1</v>
+      </c>
+      <c r="I4" s="7">
+        <v>1</v>
+      </c>
+      <c r="J4" s="7">
+        <v>1</v>
+      </c>
+      <c r="K4" s="7">
+        <v>1</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1</v>
+      </c>
+      <c r="M4" s="7">
+        <v>1</v>
+      </c>
+      <c r="N4" s="7">
+        <v>1</v>
+      </c>
+      <c r="O4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
-        <v>120</v>
-      </c>
-      <c r="D5" s="1">
-        <v>20</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="F5" s="1"/>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9">
+        <v>1</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1</v>
+      </c>
+      <c r="H5" s="7">
+        <v>1</v>
+      </c>
+      <c r="I5" s="7">
+        <v>1</v>
+      </c>
+      <c r="J5" s="7">
+        <v>1</v>
+      </c>
+      <c r="K5" s="7">
+        <v>1</v>
+      </c>
+      <c r="L5" s="7">
+        <v>1</v>
+      </c>
+      <c r="M5" s="7">
+        <v>1</v>
+      </c>
+      <c r="N5" s="7">
+        <v>1</v>
+      </c>
+      <c r="O5" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="14:14">
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="14:14">
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="14:14">
+      <c r="N19" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -635,31 +912,31 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q22" sqref="P22:Q22"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="3" max="3" width="18.5" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -673,28 +950,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -711,20 +988,20 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -732,20 +1009,20 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -764,29 +1041,29 @@
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -805,29 +1082,29 @@
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -846,29 +1123,29 @@
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1">
       <c r="A4" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1">
       <c r="A5" s="1">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
feat : PrototypeScene 수정
- 기능 합치기 1차
</commit_message>
<xml_diff>
--- a/Assets/DataTable/Data.xlsx
+++ b/Assets/DataTable/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyeon11ok\Desktop\CodeLike\Assets\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FC4914-412A-4B0D-9E0E-F793FAFFF50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B1C539-4682-458E-ACE0-FF896099855B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="818" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3727,7 +3727,7 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3894,43 +3894,43 @@
         <v>1</v>
       </c>
       <c r="C4" s="7">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="D4" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G4" s="5">
         <v>1</v>
       </c>
       <c r="H4" s="5">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I4" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J4" s="5">
         <v>1</v>
       </c>
       <c r="K4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="O4" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P4" s="24">
         <v>1</v>
@@ -3959,7 +3959,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="5">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="I5" s="5">
         <v>1</v>
@@ -3977,10 +3977,10 @@
         <v>1</v>
       </c>
       <c r="N5" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="O5" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P5" s="24">
         <v>2</v>

</xml_diff>

<commit_message>
feat:Npc 데이터 Type,shopItemIdList 추가
</commit_message>
<xml_diff>
--- a/Assets/DataTable/Data.xlsx
+++ b/Assets/DataTable/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyeon11ok\Desktop\CodeLike\Assets\DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unitywork\CodeLike\Assets\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27345FA-6439-4FEA-A534-70153A66F497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B20305-2878-4DB0-99B3-8DBCCFFDBA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3705" yWindow="2250" windowWidth="21600" windowHeight="11325" tabRatio="818" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="2340" windowWidth="20690" windowHeight="15460" tabRatio="818" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table_role" sheetId="8" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="197">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1104,6 +1104,36 @@
   </si>
   <si>
     <t>체력 회복</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shopItemIDs</t>
+  </si>
+  <si>
+    <t>List&lt;int&gt;</t>
+  </si>
+  <si>
+    <t>lee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6000,6001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6000,6001,6002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPCType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Merchant</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1436,7 +1466,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1512,6 +1542,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1820,28 +1851,28 @@
       <selection activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="3" max="3" width="13.875" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
     <col min="4" max="4" width="51" customWidth="1"/>
     <col min="7" max="7" width="17.25" customWidth="1"/>
     <col min="8" max="8" width="40.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="17.25" thickBot="1"/>
-    <row r="2" spans="2:8" ht="17.25" thickBot="1">
-      <c r="B2" s="33" t="s">
+    <row r="1" spans="2:8" ht="17.5" thickBot="1"/>
+    <row r="2" spans="2:8" ht="17.5" thickBot="1">
+      <c r="B2" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="G2" s="31" t="s">
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="G2" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="32"/>
-    </row>
-    <row r="3" spans="2:8" ht="17.25" thickBot="1">
+      <c r="H2" s="33"/>
+    </row>
+    <row r="3" spans="2:8" ht="17.5" thickBot="1">
       <c r="B3" s="12" t="s">
         <v>34</v>
       </c>
@@ -1861,7 +1892,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="2:8" ht="17.25" thickBot="1">
+    <row r="4" spans="2:8" ht="17.5" thickBot="1">
       <c r="B4" s="5">
         <v>0</v>
       </c>
@@ -1881,7 +1912,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="2:8" ht="17.25" thickBot="1">
+    <row r="5" spans="2:8" ht="17.5" thickBot="1">
       <c r="B5" s="5">
         <v>1</v>
       </c>
@@ -2125,20 +2156,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="17.25" thickBot="1"/>
-    <row r="25" spans="2:8" ht="17.25" thickBot="1">
-      <c r="B25" s="33" t="s">
+    <row r="24" spans="2:8" ht="17.5" thickBot="1"/>
+    <row r="25" spans="2:8" ht="17.5" thickBot="1">
+      <c r="B25" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="G25" s="34" t="s">
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="G25" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="H25" s="32"/>
-    </row>
-    <row r="26" spans="2:8" ht="17.25" thickBot="1">
+      <c r="H25" s="33"/>
+    </row>
+    <row r="26" spans="2:8" ht="17.5" thickBot="1">
       <c r="B26" s="12" t="s">
         <v>34</v>
       </c>
@@ -2158,7 +2189,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="17.25" thickBot="1">
+    <row r="27" spans="2:8" ht="17.5" thickBot="1">
       <c r="B27" s="5">
         <v>0</v>
       </c>
@@ -2358,8 +2389,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="2:8" ht="17.25" thickBot="1"/>
-    <row r="43" spans="2:8" ht="17.25" thickBot="1">
+    <row r="42" spans="2:8" ht="17.5" thickBot="1"/>
+    <row r="43" spans="2:8" ht="17.5" thickBot="1">
       <c r="B43" s="19" t="s">
         <v>59</v>
       </c>
@@ -2371,7 +2402,7 @@
       </c>
       <c r="H43" s="21"/>
     </row>
-    <row r="44" spans="2:8" ht="17.25" thickBot="1">
+    <row r="44" spans="2:8" ht="17.5" thickBot="1">
       <c r="B44" s="12" t="s">
         <v>34</v>
       </c>
@@ -2391,7 +2422,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="17.25" thickBot="1">
+    <row r="45" spans="2:8" ht="17.5" thickBot="1">
       <c r="B45" s="5">
         <v>0</v>
       </c>
@@ -2411,7 +2442,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="17.25" thickBot="1">
+    <row r="46" spans="2:8" ht="17.5" thickBot="1">
       <c r="B46" s="5">
         <v>1</v>
       </c>
@@ -2595,20 +2626,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="2:8" ht="17.25" thickBot="1"/>
+    <row r="60" spans="2:8" ht="17.5" thickBot="1"/>
     <row r="61" spans="2:8" ht="17.25" customHeight="1" thickBot="1">
-      <c r="B61" s="35" t="s">
+      <c r="B61" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C61" s="36"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="37"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="38"/>
       <c r="G61" s="20" t="s">
         <v>63</v>
       </c>
       <c r="H61" s="21"/>
     </row>
-    <row r="62" spans="2:8" ht="17.25" thickBot="1">
+    <row r="62" spans="2:8" ht="17.5" thickBot="1">
       <c r="B62" s="12" t="s">
         <v>34</v>
       </c>
@@ -2628,7 +2659,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="2:8" ht="17.25" thickBot="1">
+    <row r="63" spans="2:8" ht="17.5" thickBot="1">
       <c r="B63" s="5">
         <v>0</v>
       </c>
@@ -2648,7 +2679,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="2:8" ht="17.25" thickBot="1">
+    <row r="64" spans="2:8" ht="17.5" thickBot="1">
       <c r="B64" s="5">
         <v>1</v>
       </c>
@@ -2668,7 +2699,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="2:8" ht="17.25" thickBot="1">
+    <row r="65" spans="2:8" ht="17.5" thickBot="1">
       <c r="B65" s="5">
         <v>2</v>
       </c>
@@ -2838,20 +2869,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="2:8" ht="17.25" thickBot="1"/>
-    <row r="79" spans="2:8" ht="17.25" thickBot="1">
-      <c r="B79" s="35" t="s">
+    <row r="78" spans="2:8" ht="17.5" thickBot="1"/>
+    <row r="79" spans="2:8" ht="17.5" thickBot="1">
+      <c r="B79" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="C79" s="36"/>
-      <c r="D79" s="36"/>
-      <c r="E79" s="37"/>
+      <c r="C79" s="37"/>
+      <c r="D79" s="37"/>
+      <c r="E79" s="38"/>
       <c r="G79" s="20" t="s">
         <v>65</v>
       </c>
       <c r="H79" s="21"/>
     </row>
-    <row r="80" spans="2:8" ht="17.25" thickBot="1">
+    <row r="80" spans="2:8" ht="17.5" thickBot="1">
       <c r="B80" s="12" t="s">
         <v>34</v>
       </c>
@@ -2871,7 +2902,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="2:8" ht="17.25" thickBot="1">
+    <row r="81" spans="2:8" ht="17.5" thickBot="1">
       <c r="B81" s="5">
         <v>0</v>
       </c>
@@ -2891,7 +2922,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="82" spans="2:8" ht="17.25" thickBot="1">
+    <row r="82" spans="2:8" ht="17.5" thickBot="1">
       <c r="B82" s="5">
         <v>1</v>
       </c>
@@ -2911,7 +2942,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="2:8" ht="17.25" thickBot="1">
+    <row r="83" spans="2:8" ht="17.5" thickBot="1">
       <c r="B83" s="5">
         <v>2</v>
       </c>
@@ -3081,20 +3112,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="96" spans="2:8" ht="17.25" thickBot="1"/>
-    <row r="97" spans="2:8" ht="17.25" thickBot="1">
-      <c r="B97" s="35" t="s">
+    <row r="96" spans="2:8" ht="17.5" thickBot="1"/>
+    <row r="97" spans="2:8" ht="17.5" thickBot="1">
+      <c r="B97" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="C97" s="36"/>
-      <c r="D97" s="36"/>
-      <c r="E97" s="37"/>
+      <c r="C97" s="37"/>
+      <c r="D97" s="37"/>
+      <c r="E97" s="38"/>
       <c r="G97" s="20" t="s">
         <v>65</v>
       </c>
       <c r="H97" s="21"/>
     </row>
-    <row r="98" spans="2:8" ht="17.25" thickBot="1">
+    <row r="98" spans="2:8" ht="17.5" thickBot="1">
       <c r="B98" s="12" t="s">
         <v>34</v>
       </c>
@@ -3114,7 +3145,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="99" spans="2:8" ht="17.25" thickBot="1">
+    <row r="99" spans="2:8" ht="17.5" thickBot="1">
       <c r="B99" s="5">
         <v>0</v>
       </c>
@@ -3134,7 +3165,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="100" spans="2:8" ht="17.25" thickBot="1">
+    <row r="100" spans="2:8" ht="17.5" thickBot="1">
       <c r="B100" s="5">
         <v>1</v>
       </c>
@@ -3154,7 +3185,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="101" spans="2:8" ht="17.25" thickBot="1">
+    <row r="101" spans="2:8" ht="17.5" thickBot="1">
       <c r="B101" s="5">
         <v>2</v>
       </c>
@@ -3324,20 +3355,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="114" spans="2:8" ht="17.25" thickBot="1"/>
-    <row r="115" spans="2:8" ht="17.25" thickBot="1">
-      <c r="B115" s="35" t="s">
+    <row r="114" spans="2:8" ht="17.5" thickBot="1"/>
+    <row r="115" spans="2:8" ht="17.5" thickBot="1">
+      <c r="B115" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C115" s="36"/>
-      <c r="D115" s="36"/>
-      <c r="E115" s="37"/>
+      <c r="C115" s="37"/>
+      <c r="D115" s="37"/>
+      <c r="E115" s="38"/>
       <c r="G115" s="20" t="s">
         <v>67</v>
       </c>
       <c r="H115" s="21"/>
     </row>
-    <row r="116" spans="2:8" ht="17.25" thickBot="1">
+    <row r="116" spans="2:8" ht="17.5" thickBot="1">
       <c r="B116" s="12" t="s">
         <v>34</v>
       </c>
@@ -3357,7 +3388,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="117" spans="2:8" ht="17.25" thickBot="1">
+    <row r="117" spans="2:8" ht="17.5" thickBot="1">
       <c r="B117" s="5">
         <v>0</v>
       </c>
@@ -3576,42 +3607,74 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53829A82-7AF8-4424-A74D-079B89F0926D}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
+  <cols>
+    <col min="3" max="3" width="16.58203125" style="31" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="D1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>8000</v>
       </c>
       <c r="B3" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C3" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="D3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>8001</v>
+      </c>
+      <c r="B4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="D4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
     </row>
   </sheetData>
@@ -3628,9 +3691,9 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="3" max="3" width="14.125" customWidth="1"/>
+    <col min="3" max="3" width="14.08203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3767,7 +3830,7 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="3" max="3" width="12.75" customWidth="1"/>
@@ -4023,14 +4086,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="5" max="5" width="21.875" customWidth="1"/>
-    <col min="6" max="7" width="18.375" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+    <col min="6" max="7" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -4390,12 +4453,12 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="3" max="3" width="18.5" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="23.125" customWidth="1"/>
-    <col min="6" max="6" width="18.375" customWidth="1"/>
+    <col min="5" max="5" width="23.08203125" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -4496,16 +4559,16 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="16.58203125" customWidth="1"/>
     <col min="3" max="3" width="13.75" customWidth="1"/>
-    <col min="4" max="4" width="17.125" customWidth="1"/>
-    <col min="5" max="5" width="16.875" customWidth="1"/>
-    <col min="6" max="6" width="16.375" customWidth="1"/>
+    <col min="4" max="4" width="17.08203125" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" customWidth="1"/>
     <col min="7" max="7" width="45.75" customWidth="1"/>
     <col min="8" max="8" width="15.25" customWidth="1"/>
-    <col min="9" max="9" width="15.625" customWidth="1"/>
+    <col min="9" max="9" width="15.58203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -4660,11 +4723,11 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="5" max="5" width="29.625" customWidth="1"/>
-    <col min="6" max="6" width="16.125" customWidth="1"/>
+    <col min="5" max="5" width="29.58203125" customWidth="1"/>
+    <col min="6" max="6" width="16.08203125" customWidth="1"/>
     <col min="9" max="10" width="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4728,7 +4791,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="49.5">
+    <row r="4" spans="1:6" ht="51">
       <c r="A4" s="1">
         <v>4001</v>
       </c>
@@ -4748,7 +4811,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="17.25">
+    <row r="5" spans="1:6" ht="17.5">
       <c r="A5" s="1"/>
       <c r="E5" s="29"/>
       <c r="F5" s="30"/>
@@ -4767,14 +4830,14 @@
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
     <col min="7" max="7" width="17.5" customWidth="1"/>
     <col min="8" max="8" width="14.5" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="20.125" customWidth="1"/>
+    <col min="10" max="10" width="20.08203125" customWidth="1"/>
     <col min="11" max="11" width="18.75" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
   </cols>
@@ -4997,14 +5060,14 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="23.375" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.25" customWidth="1"/>
-    <col min="6" max="6" width="38.125" customWidth="1"/>
-    <col min="7" max="7" width="24.625" customWidth="1"/>
+    <col min="6" max="6" width="38.08203125" customWidth="1"/>
+    <col min="7" max="7" width="24.58203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -5167,12 +5230,12 @@
       <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="22.375" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="4" max="4" width="19.75" customWidth="1"/>
-    <col min="5" max="5" width="29.125" customWidth="1"/>
+    <col min="5" max="5" width="29.08203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>

<commit_message>
feat: 힐러 NPC 추가
-NPC 오브젝트 하나당 힐 한번만 가능하도록 설정
- 0~100% 랜덤으로 치유
- 게임매니저 리팩토링
</commit_message>
<xml_diff>
--- a/Assets/DataTable/Data.xlsx
+++ b/Assets/DataTable/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\unitywork\CodeLike\Assets\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA2F7AE-92E6-452F-B342-7091C60D6C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2EA88B6-8D50-4F1F-8E6D-55F1D283C0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21300" yWindow="0" windowWidth="16780" windowHeight="11150" tabRatio="818" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="223">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1232,6 +1232,10 @@
   </si>
   <si>
     <t>Enhancer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Healer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5810,7 +5814,7 @@
         <v>220</v>
       </c>
       <c r="D6" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat : Npc 데이터 수정
</commit_message>
<xml_diff>
--- a/Assets/DataTable/Data.xlsx
+++ b/Assets/DataTable/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyeon11ok\Desktop\CodeLike\Assets\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1049A053-A860-4688-B427-FB60364D5CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DA66A3-1C07-450C-88C5-0486D1E259C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="818" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="818" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table_role" sheetId="8" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="218">
   <si>
     <t>int</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -903,26 +903,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>첫문장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>두문장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>세문장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>네문장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>다섯문장</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>sellPrice</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -969,21 +949,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>shopItemIDs</t>
-  </si>
-  <si>
     <t>lee</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>6000,6001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>6000,6001,6002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Type</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1017,10 +986,6 @@
   </si>
   <si>
     <t>Fire Zone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>List&lt;int&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1576,7 +1541,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1651,7 +1616,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1979,16 +1943,16 @@
   <sheetData>
     <row r="1" spans="2:8" ht="17.25" thickBot="1"/>
     <row r="2" spans="2:8" ht="17.25" thickBot="1">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="G2" s="34" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="G2" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="35"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="2:8" ht="17.25" thickBot="1">
       <c r="B3" s="12" t="s">
@@ -2276,16 +2240,16 @@
     </row>
     <row r="24" spans="2:8" ht="17.25" thickBot="1"/>
     <row r="25" spans="2:8" ht="17.25" thickBot="1">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="G25" s="37" t="s">
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="G25" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="H25" s="35"/>
+      <c r="H25" s="34"/>
     </row>
     <row r="26" spans="2:8" ht="17.25" thickBot="1">
       <c r="B26" s="12" t="s">
@@ -2746,12 +2710,12 @@
     </row>
     <row r="60" spans="2:8" ht="17.25" thickBot="1"/>
     <row r="61" spans="2:8" ht="17.25" customHeight="1" thickBot="1">
-      <c r="B61" s="38" t="s">
+      <c r="B61" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="40"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="38"/>
+      <c r="E61" s="39"/>
       <c r="G61" s="20" t="s">
         <v>56</v>
       </c>
@@ -2989,12 +2953,12 @@
     </row>
     <row r="78" spans="2:8" ht="17.25" thickBot="1"/>
     <row r="79" spans="2:8" ht="17.25" thickBot="1">
-      <c r="B79" s="38" t="s">
+      <c r="B79" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C79" s="39"/>
-      <c r="D79" s="39"/>
-      <c r="E79" s="40"/>
+      <c r="C79" s="38"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="39"/>
       <c r="G79" s="20" t="s">
         <v>58</v>
       </c>
@@ -3232,12 +3196,12 @@
     </row>
     <row r="96" spans="2:8" ht="17.25" thickBot="1"/>
     <row r="97" spans="2:8" ht="17.25" thickBot="1">
-      <c r="B97" s="38" t="s">
+      <c r="B97" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C97" s="39"/>
-      <c r="D97" s="39"/>
-      <c r="E97" s="40"/>
+      <c r="C97" s="38"/>
+      <c r="D97" s="38"/>
+      <c r="E97" s="39"/>
       <c r="G97" s="20" t="s">
         <v>58</v>
       </c>
@@ -3475,12 +3439,12 @@
     </row>
     <row r="114" spans="2:8" ht="17.25" thickBot="1"/>
     <row r="115" spans="2:8" ht="17.25" thickBot="1">
-      <c r="B115" s="38" t="s">
+      <c r="B115" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C115" s="39"/>
-      <c r="D115" s="39"/>
-      <c r="E115" s="40"/>
+      <c r="C115" s="38"/>
+      <c r="D115" s="38"/>
+      <c r="E115" s="39"/>
       <c r="G115" s="20" t="s">
         <v>60</v>
       </c>
@@ -3768,7 +3732,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B3">
         <v>101</v>
@@ -3782,7 +3746,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B4">
         <v>102</v>
@@ -3796,7 +3760,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B5">
         <v>103</v>
@@ -3810,7 +3774,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B6">
         <v>104</v>
@@ -3942,10 +3906,10 @@
         <v>503</v>
       </c>
       <c r="C15" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D15" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3956,10 +3920,10 @@
         <v>504</v>
       </c>
       <c r="C16" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D16" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -4021,7 +3985,7 @@
         <v>39</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="N1" s="9" t="s">
         <v>22</v>
@@ -4336,7 +4300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF2F1DE-C499-42C0-9AF5-F928DBDC5D56}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -4394,7 +4358,7 @@
         <v>4000</v>
       </c>
       <c r="B3" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C3">
         <v>301</v>
@@ -4403,51 +4367,51 @@
         <v>5000</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="F3" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A4" s="32">
+      <c r="A4" s="31">
         <v>4001</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>221</v>
-      </c>
-      <c r="C4" s="31">
+        <v>212</v>
+      </c>
+      <c r="C4" s="30">
         <v>301</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="30">
         <v>5001</v>
       </c>
-      <c r="E4" s="33" t="s">
-        <v>220</v>
-      </c>
-      <c r="F4" s="31" t="s">
-        <v>224</v>
-      </c>
-      <c r="G4" s="31"/>
+      <c r="E4" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>215</v>
+      </c>
+      <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
         <v>4002</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C5">
         <v>301</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="30">
         <v>5003</v>
       </c>
       <c r="E5" t="s">
-        <v>219</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>225</v>
+        <v>210</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -4455,7 +4419,7 @@
         <v>4003</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C6">
         <v>301</v>
@@ -4464,10 +4428,10 @@
         <v>5002</v>
       </c>
       <c r="E6" t="s">
-        <v>191</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>226</v>
+        <v>182</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -4519,10 +4483,10 @@
         <v>117</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>11</v>
@@ -4566,7 +4530,7 @@
         <v>5000</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C3" s="28">
         <v>501</v>
@@ -4584,10 +4548,10 @@
         <v>6</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -4595,7 +4559,7 @@
         <v>5001</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C4" s="28">
         <v>502</v>
@@ -4613,10 +4577,10 @@
         <v>6</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="J4" s="29" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -4624,7 +4588,7 @@
         <v>5002</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C5" s="28">
         <v>503</v>
@@ -4642,10 +4606,10 @@
         <v>6</v>
       </c>
       <c r="H5" s="29" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -4653,7 +4617,7 @@
         <v>5003</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C6" s="28">
         <v>504</v>
@@ -4671,10 +4635,10 @@
         <v>6</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="J6" s="29" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -4724,10 +4688,10 @@
         <v>134</v>
       </c>
       <c r="H1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="I1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -4785,7 +4749,7 @@
         <v>200</v>
       </c>
       <c r="I3" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -4814,7 +4778,7 @@
         <v>100</v>
       </c>
       <c r="I4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -4822,7 +4786,7 @@
         <v>6002</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C5">
         <v>301</v>
@@ -4834,16 +4798,16 @@
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="H5">
         <v>300</v>
       </c>
       <c r="I5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -4883,19 +4847,19 @@
         <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="E1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="F1" t="s">
         <v>131</v>
       </c>
       <c r="G1" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="H1" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -4918,10 +4882,10 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="H2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -4929,7 +4893,7 @@
         <v>7000</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -4941,13 +4905,13 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="G3" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="H3" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -4955,7 +4919,7 @@
         <v>7001</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -4967,13 +4931,13 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G4" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="H4" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -4981,7 +4945,7 @@
         <v>7002</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C5" t="s">
         <v>94</v>
@@ -4993,13 +4957,13 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="G5" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="H5" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -5007,7 +4971,7 @@
         <v>7003</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
@@ -5019,13 +4983,13 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="G6" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="H6" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -5033,7 +4997,7 @@
         <v>7004</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C7" t="s">
         <v>114</v>
@@ -5045,13 +5009,13 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="G7" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="H7" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -5059,10 +5023,10 @@
         <v>7005</v>
       </c>
       <c r="B8" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C8" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D8">
         <v>0.3</v>
@@ -5071,13 +5035,13 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="G8" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="H8" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -5085,7 +5049,7 @@
         <v>7006</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -5097,13 +5061,13 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="G9" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="H9" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -5111,7 +5075,7 @@
         <v>7007</v>
       </c>
       <c r="B10" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C10" t="s">
         <v>21</v>
@@ -5123,13 +5087,13 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="G10" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="H10" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -5693,145 +5657,87 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53829A82-7AF8-4424-A74D-079B89F0926D}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="3" max="3" width="16.625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="30" t="s">
-        <v>155</v>
+      <c r="C1" t="s">
+        <v>151</v>
       </c>
       <c r="D1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E1" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="30" t="s">
-        <v>168</v>
+      <c r="C2" t="s">
+        <v>152</v>
       </c>
       <c r="D2" t="s">
         <v>160</v>
       </c>
-      <c r="E2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>8000</v>
       </c>
       <c r="B3" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="D3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F3" t="s">
-        <v>139</v>
-      </c>
-      <c r="G3" t="s">
-        <v>140</v>
-      </c>
-      <c r="H3" t="s">
-        <v>141</v>
-      </c>
-      <c r="I3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="C3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>8001</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="D4" t="s">
-        <v>161</v>
-      </c>
-      <c r="E4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F4" t="s">
-        <v>139</v>
-      </c>
-      <c r="G4" t="s">
-        <v>140</v>
-      </c>
-      <c r="H4" t="s">
-        <v>141</v>
-      </c>
-      <c r="I4" t="s">
-        <v>142</v>
-      </c>
-      <c r="J4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K4" t="s">
-        <v>139</v>
-      </c>
-      <c r="L4" t="s">
-        <v>140</v>
-      </c>
-      <c r="M4" t="s">
-        <v>141</v>
-      </c>
-      <c r="N4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>150</v>
+      </c>
+      <c r="C4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>8002</v>
       </c>
       <c r="B5" t="s">
-        <v>190</v>
-      </c>
-      <c r="D5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>181</v>
+      </c>
+      <c r="C5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>8003</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
-      </c>
-      <c r="D6" t="s">
-        <v>217</v>
+        <v>206</v>
+      </c>
+      <c r="C6" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat : 플레이어 EnegyWave 탄속 상승
</commit_message>
<xml_diff>
--- a/Assets/DataTable/Data.xlsx
+++ b/Assets/DataTable/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity\CodeLike\Assets\DataTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyeon11ok\Desktop\CodeLike\Assets\DataTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5320FB4A-8623-4764-958F-C293AD622000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62A6B12-A3A9-4C8A-BA0C-0444CF857E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="818" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1920" windowWidth="21600" windowHeight="11325" tabRatio="818" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table_role" sheetId="8" r:id="rId1"/>
@@ -4151,7 +4151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
@@ -4752,8 +4752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE846C94-81F7-444B-B5AD-705320432DBD}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -4847,7 +4847,7 @@
         <v>60</v>
       </c>
       <c r="E3" s="29">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F3" s="29">
         <v>0</v>

</xml_diff>